<commit_message>
Fix Gantt: Use hardcoded data for reliability; sprint view
</commit_message>
<xml_diff>
--- a/pilot_gantt_chart_sprints.xlsx
+++ b/pilot_gantt_chart_sprints.xlsx
@@ -49,26 +49,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="004F81BD"/>
-        <bgColor rgb="004F81BD"/>
+        <fgColor rgb="00002060"/>
+        <bgColor rgb="00002060"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00A52A2A"/>
-        <bgColor rgb="00A52A2A"/>
+        <fgColor rgb="00C00000"/>
+        <bgColor rgb="00C00000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00228B22"/>
-        <bgColor rgb="00228B22"/>
+        <fgColor rgb="0000B050"/>
+        <bgColor rgb="0000B050"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00B4C6E7"/>
-        <bgColor rgb="00B4C6E7"/>
+        <fgColor rgb="00AEAAAA"/>
+        <bgColor rgb="00AEAAAA"/>
       </patternFill>
     </fill>
   </fills>
@@ -476,19 +476,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="100" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="16" customWidth="1" min="3" max="3"/>
-    <col width="16" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="16" customWidth="1" min="6" max="6"/>
-    <col width="16" customWidth="1" min="7" max="7"/>
-    <col width="16" customWidth="1" min="8" max="8"/>
-    <col width="16" customWidth="1" min="9" max="9"/>
-    <col width="16" customWidth="1" min="10" max="10"/>
-    <col width="16" customWidth="1" min="11" max="11"/>
-    <col width="16" customWidth="1" min="12" max="12"/>
-    <col width="16" customWidth="1" min="13" max="13"/>
+    <col width="105" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1" ht="45" customHeight="1">
@@ -499,62 +499,74 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>Sprint 1 (W1-2)</t>
+          <t>Sprint 1
+(W1-W2)</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>Sprint 2 (W3-4)</t>
+          <t>Sprint 2
+(W3-W4)</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Sprint 3 (W5-6)</t>
+          <t>Sprint 3
+(W5-W6)</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Sprint 4 (W7-8)</t>
+          <t>Sprint 4
+(W7-W8)</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>Sprint 5 (W9-10)</t>
+          <t>Sprint 5
+(W9-W10)</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>Sprint 6 (W11-12)</t>
+          <t>Sprint 6
+(W11-W12)</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Sprint 7 (W13-14)</t>
+          <t>Sprint 7
+(W13-W14)</t>
         </is>
       </c>
       <c r="I1" s="2" t="inlineStr">
         <is>
-          <t>Sprint 8 (W15-16)</t>
+          <t>Sprint 8
+(W15-W16)</t>
         </is>
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>Sprint 9 (W17-18)</t>
+          <t>Sprint 9
+(W17-W18)</t>
         </is>
       </c>
       <c r="K1" s="2" t="inlineStr">
         <is>
-          <t>Sprint 10 (W19-20)</t>
+          <t>Sprint 10
+(W19-W20)</t>
         </is>
       </c>
       <c r="L1" s="2" t="inlineStr">
         <is>
-          <t>Sprint 11 (W21-22)</t>
+          <t>Sprint 11
+(W21-W22)</t>
         </is>
       </c>
       <c r="M1" s="2" t="inlineStr">
         <is>
-          <t>Sprint 12 (W23-24)</t>
+          <t>Sprint 12
+(W23-W24)</t>
         </is>
       </c>
     </row>
@@ -568,93 +580,119 @@
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>Discovery, Analysis &amp; Planning</t>
+          <t>Phase 1: Discovery, Analysis &amp; Planning (Est. Months 1-2)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>1. Deep Dive into Existing UAT Processes &amp; Test Assets</t>
-        </is>
-      </c>
+          <t>1. Deep Dive into Existing UAT Processes &amp; Test Assets (W1-W3)</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="n"/>
+      <c r="C4" s="6" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>2. Identify &amp; Prioritize UAT Scenarios for Automation</t>
-        </is>
-      </c>
+          <t>2. Identify &amp; Prioritize UAT Scenarios for Automation (W3-W6)</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="n"/>
+      <c r="D5" s="6" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>3. Master BDD Tooling &amp; Methodology</t>
-        </is>
-      </c>
+          <t>3. Master BDD Tooling &amp; Methodology (W2-W5)</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="n"/>
+      <c r="C6" s="6" t="n"/>
+      <c r="D6" s="6" t="n"/>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>Migration, Automation Development &amp; Initial Integration</t>
+          <t>Phase 2: Migration, Automation Development &amp; Initial Integration (Est. Months 3-4)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>4. Convert Selected UAT Scenarios to BDD (Gherkin)</t>
-        </is>
-      </c>
+          <t>4. Convert Selected UAT Scenarios to BDD (Gherkin) (W7-W10)</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="n"/>
+      <c r="F8" s="6" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="inlineStr">
         <is>
-          <t>5. Develop Automated Test Scripts using Playwright</t>
-        </is>
-      </c>
+          <t>5. Develop Automated Test Scripts using Playwright (W9-W16)</t>
+        </is>
+      </c>
+      <c r="F9" s="6" t="n"/>
+      <c r="G9" s="6" t="n"/>
+      <c r="H9" s="6" t="n"/>
+      <c r="I9" s="6" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="inlineStr">
         <is>
-          <t>6. Setup &amp; Test Execution in DT2 Environment</t>
-        </is>
-      </c>
+          <t>6. Setup &amp; Test Execution in DT2 Environment (W15-W18)</t>
+        </is>
+      </c>
+      <c r="I10" s="6" t="n"/>
+      <c r="J10" s="6" t="n"/>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>Refinement, Reporting &amp; Knowledge Transfer Preparation</t>
+          <t>Phase 3: Refinement, Reporting &amp; Knowledge Transfer Preparation (Est. Months 5-6)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="inlineStr">
         <is>
-          <t>7. Iterate and Refine Automated UAT Suite</t>
-        </is>
-      </c>
+          <t>7. Iterate and Refine Automated UAT Suite (W17-W24)</t>
+        </is>
+      </c>
+      <c r="J12" s="6" t="n"/>
+      <c r="K12" s="6" t="n"/>
+      <c r="L12" s="6" t="n"/>
+      <c r="M12" s="6" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="inlineStr">
         <is>
-          <t>8. Establish Automated UAT Reporting</t>
-        </is>
-      </c>
+          <t>8. Establish Automated UAT Reporting (W19-W22)</t>
+        </is>
+      </c>
+      <c r="K13" s="6" t="n"/>
+      <c r="L13" s="6" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="inlineStr">
         <is>
-          <t>9. Document Best Practices &amp; Create Migration Playbook</t>
-        </is>
-      </c>
+          <t>9. Document Best Practices &amp; Create Migration Playbook (W20-W24)</t>
+        </is>
+      </c>
+      <c r="K14" s="6" t="n"/>
+      <c r="L14" s="6" t="n"/>
+      <c r="M14" s="6" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="inlineStr">
         <is>
-          <t>10. Prepare for Knowledge Sharing &amp; Team Onboarding</t>
-        </is>
-      </c>
+          <t>10. Prepare for Knowledge Sharing &amp; Team Onboarding (W22-W24)</t>
+        </is>
+      </c>
+      <c r="L15" s="6" t="n"/>
+      <c r="M15" s="6" t="n"/>
     </row>
     <row r="16" ht="22" customHeight="1">
       <c r="A16" s="3" t="inlineStr">
@@ -666,72 +704,95 @@
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>Assessment, Strategy Definition &amp; Foundational Setup</t>
+          <t>Phase 1: Assessment, Strategy Definition &amp; Foundational Setup (Est. Months 1-2)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="inlineStr">
         <is>
-          <t>1. Baseline Current Engineering Practices &amp; CI/CD Maturity</t>
-        </is>
-      </c>
+          <t>1. Baseline Current Engineering Practices &amp; CI/CD Maturity (W1-W3)</t>
+        </is>
+      </c>
+      <c r="B18" s="6" t="n"/>
+      <c r="C18" s="6" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>2. Develop &amp; Communicate Pilot Engineering Practices Adoption Strategy</t>
-        </is>
-      </c>
+          <t>2. Develop &amp; Communicate Pilot Engineering Practices Adoption Strategy (W2-W4)</t>
+        </is>
+      </c>
+      <c r="B19" s="6" t="n"/>
+      <c r="C19" s="6" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>3. Tooling Onboarding &amp; Environment Preparation</t>
-        </is>
-      </c>
+          <t>3. Tooling Onboarding &amp; Environment Preparation (W3-W6)</t>
+        </is>
+      </c>
+      <c r="C20" s="6" t="n"/>
+      <c r="D20" s="6" t="n"/>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Implementation, Coaching &amp; CI/CD Integration</t>
+          <t>Phase 2: Implementation, Coaching &amp; CI/CD Integration (Est. Months 3-4)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="inlineStr">
         <is>
-          <t>4. Drive Adoption of Unit Testing &amp; Developer-Led Testing</t>
-        </is>
-      </c>
+          <t>4. Drive Adoption of Unit Testing &amp; Developer-Led Testing (W7-W16)</t>
+        </is>
+      </c>
+      <c r="E22" s="6" t="n"/>
+      <c r="F22" s="6" t="n"/>
+      <c r="G22" s="6" t="n"/>
+      <c r="H22" s="6" t="n"/>
+      <c r="I22" s="6" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="inlineStr">
         <is>
-          <t>5. Integrate Automated Tests into CI/CD Pipelines (GitHub Actions Focus)</t>
-        </is>
-      </c>
+          <t>5. Integrate Automated Tests into CI/CD Pipelines (GitHub Actions Focus) (W9-W16)</t>
+        </is>
+      </c>
+      <c r="F23" s="6" t="n"/>
+      <c r="G23" s="6" t="n"/>
+      <c r="H23" s="6" t="n"/>
+      <c r="I23" s="6" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="inlineStr">
         <is>
-          <t>6. Establish &amp; Champion Mocking Practices (Mockito/MockFlow)</t>
-        </is>
-      </c>
+          <t>6. Establish &amp; Champion Mocking Practices (Mockito/MockFlow) (W10-W15)</t>
+        </is>
+      </c>
+      <c r="F24" s="6" t="n"/>
+      <c r="G24" s="6" t="n"/>
+      <c r="H24" s="6" t="n"/>
+      <c r="I24" s="6" t="n"/>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>Optimization, Standardization &amp; Knowledge Dissemination</t>
+          <t>Phase 3: Optimization, Standardization &amp; Knowledge Dissemination (Est. Months 5-6)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="inlineStr">
         <is>
-          <t>7. Refine CI/CD Pipelines (GitHub Actions) and Test Execution Efficiency</t>
-        </is>
-      </c>
+          <t>7. Refine CI/CD Pipelines (GitHub Actions) and Test Execution Efficiency (W17-W24)</t>
+        </is>
+      </c>
+      <c r="J26" s="6" t="n"/>
+      <c r="K26" s="6" t="n"/>
+      <c r="L26" s="6" t="n"/>
+      <c r="M26" s="6" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="inlineStr">
@@ -747,16 +808,21 @@
     <row r="28">
       <c r="A28" s="5" t="inlineStr">
         <is>
-          <t>9. Facilitate Performance Profiling Setup</t>
-        </is>
-      </c>
+          <t>9. Facilitate Performance Profiling Setup (W20-W23)</t>
+        </is>
+      </c>
+      <c r="K28" s="6" t="n"/>
+      <c r="L28" s="6" t="n"/>
+      <c r="M28" s="6" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="inlineStr">
         <is>
-          <t>10. Prepare for Scaling &amp; Knowledge Transfer</t>
-        </is>
-      </c>
+          <t>10. Prepare for Scaling &amp; Knowledge Transfer (W22-W24)</t>
+        </is>
+      </c>
+      <c r="L29" s="6" t="n"/>
+      <c r="M29" s="6" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>